<commit_message>
2015/08/03 Update IT ST
</commit_message>
<xml_diff>
--- a/WIP/Users/HieuTM/20150728_SysTestcase_HieuTM.xlsx
+++ b/WIP/Users/HieuTM/20150728_SysTestcase_HieuTM.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6555" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6555"/>
   </bookViews>
   <sheets>
     <sheet name="Common" sheetId="1" r:id="rId1"/>
     <sheet name="User" sheetId="2" r:id="rId2"/>
+    <sheet name="Non-functional" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -80,8 +81,36 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="F8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="8"/>
+            <rFont val="Times New Roman"/>
+            <family val="1"/>
+          </rPr>
+          <t xml:space="preserve">Pass
+Fail
+Untested
+N/A
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="227">
   <si>
     <t>Module Code</t>
   </si>
@@ -1282,6 +1311,46 @@
   <si>
     <t>1. Create Post panel is displayed
 2. Create Post panel is closed</t>
+  </si>
+  <si>
+    <t>1. Homepage is displayed
+2. Login form is displayed
+3. "user1@gmail.com" is displayed in user name text box
+•••••••••••• is displayed in password text box
+4. User is logged in. Homepage is displayed after at most 5 second</t>
+  </si>
+  <si>
+    <t>1. Search page is displayed after at most 5 seconds</t>
+  </si>
+  <si>
+    <t>1. Friend menu is displayed after at most 5 seconds</t>
+  </si>
+  <si>
+    <t>1. Notification menu is displayed after at most 5 seconds</t>
+  </si>
+  <si>
+    <t>1. Message menu is displayed after at most 5 seconds</t>
+  </si>
+  <si>
+    <t>1. User menu is displayed after at most 5 seconds</t>
+  </si>
+  <si>
+    <t>1. Homepage is displayed after at most 5 seconds</t>
+  </si>
+  <si>
+    <t>1. Hompage is displayed after at most 5 seconds</t>
+  </si>
+  <si>
+    <t>1. Buttons are displayed after at most 5 seconds</t>
+  </si>
+  <si>
+    <t>1. Post page is displayed after at most 5 seconds</t>
+  </si>
+  <si>
+    <t>1. Create Post panel is displayed after at most 5 seconds</t>
+  </si>
+  <si>
+    <t>1. Reload Homepage. Homepage is displayed after at most 5 seconds</t>
   </si>
 </sst>
 </file>
@@ -1878,7 +1947,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2134,6 +2203,24 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2142,6 +2229,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2151,6 +2247,15 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2178,15 +2283,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2196,32 +2292,36 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2507,7 +2607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2907,9 +3007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
-    </sheetView>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3043,15 +3141,15 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="11"/>
-      <c r="B9" s="96" t="s">
+      <c r="B9" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="97"/>
-      <c r="D9" s="97"/>
-      <c r="E9" s="97"/>
-      <c r="F9" s="97"/>
-      <c r="G9" s="97"/>
-      <c r="H9" s="98"/>
+      <c r="C9" s="109"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="110"/>
     </row>
     <row r="10" spans="1:8" ht="76.5">
       <c r="A10" s="50" t="s">
@@ -3075,10 +3173,10 @@
       <c r="A11" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="120" t="s">
         <v>77</v>
       </c>
       <c r="D11" s="49" t="s">
@@ -3095,10 +3193,10 @@
       <c r="A12" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="53" t="s">
         <v>84</v>
       </c>
       <c r="D12" s="51" t="s">
@@ -3115,7 +3213,7 @@
       <c r="A13" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="43" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="24" t="s">
@@ -3173,15 +3271,15 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="46"/>
-      <c r="B16" s="108" t="s">
+      <c r="B16" s="117" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="109"/>
-      <c r="D16" s="109"/>
-      <c r="E16" s="109"/>
-      <c r="F16" s="109"/>
-      <c r="G16" s="109"/>
-      <c r="H16" s="110"/>
+      <c r="C16" s="118"/>
+      <c r="D16" s="118"/>
+      <c r="E16" s="118"/>
+      <c r="F16" s="118"/>
+      <c r="G16" s="118"/>
+      <c r="H16" s="119"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="62" t="s">
@@ -3383,15 +3481,15 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="63"/>
-      <c r="B28" s="93" t="s">
+      <c r="B28" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="94"/>
-      <c r="D28" s="94"/>
-      <c r="E28" s="94"/>
-      <c r="F28" s="94"/>
-      <c r="G28" s="94"/>
-      <c r="H28" s="95"/>
+      <c r="C28" s="103"/>
+      <c r="D28" s="103"/>
+      <c r="E28" s="103"/>
+      <c r="F28" s="103"/>
+      <c r="G28" s="103"/>
+      <c r="H28" s="104"/>
     </row>
     <row r="29" spans="1:8" ht="14.25" customHeight="1">
       <c r="A29" s="57"/>
@@ -3449,15 +3547,15 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="31"/>
-      <c r="B32" s="99" t="s">
+      <c r="B32" s="111" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="100"/>
-      <c r="D32" s="100"/>
-      <c r="E32" s="100"/>
-      <c r="F32" s="100"/>
-      <c r="G32" s="100"/>
-      <c r="H32" s="101"/>
+      <c r="C32" s="112"/>
+      <c r="D32" s="112"/>
+      <c r="E32" s="112"/>
+      <c r="F32" s="112"/>
+      <c r="G32" s="112"/>
+      <c r="H32" s="113"/>
     </row>
     <row r="33" spans="1:8" ht="140.25">
       <c r="A33" s="31" t="s">
@@ -3499,15 +3597,15 @@
     </row>
     <row r="35" spans="1:8" ht="12.75" customHeight="1">
       <c r="A35" s="31"/>
-      <c r="B35" s="99" t="s">
+      <c r="B35" s="111" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="100"/>
-      <c r="D35" s="100"/>
-      <c r="E35" s="100"/>
-      <c r="F35" s="100"/>
-      <c r="G35" s="100"/>
-      <c r="H35" s="101"/>
+      <c r="C35" s="112"/>
+      <c r="D35" s="112"/>
+      <c r="E35" s="112"/>
+      <c r="F35" s="112"/>
+      <c r="G35" s="112"/>
+      <c r="H35" s="113"/>
     </row>
     <row r="36" spans="1:8" ht="14.25" customHeight="1">
       <c r="A36" s="62" t="s">
@@ -3777,15 +3875,15 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="31"/>
-      <c r="B51" s="102" t="s">
+      <c r="B51" s="114" t="s">
         <v>51</v>
       </c>
-      <c r="C51" s="103"/>
-      <c r="D51" s="103"/>
-      <c r="E51" s="103"/>
-      <c r="F51" s="103"/>
-      <c r="G51" s="103"/>
-      <c r="H51" s="104"/>
+      <c r="C51" s="115"/>
+      <c r="D51" s="115"/>
+      <c r="E51" s="115"/>
+      <c r="F51" s="115"/>
+      <c r="G51" s="115"/>
+      <c r="H51" s="116"/>
     </row>
     <row r="52" spans="1:8" ht="140.25">
       <c r="A52" s="31" t="s">
@@ -3917,15 +4015,15 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="31"/>
-      <c r="B59" s="99" t="s">
+      <c r="B59" s="111" t="s">
         <v>52</v>
       </c>
-      <c r="C59" s="100"/>
-      <c r="D59" s="100"/>
-      <c r="E59" s="100"/>
-      <c r="F59" s="100"/>
-      <c r="G59" s="100"/>
-      <c r="H59" s="101"/>
+      <c r="C59" s="112"/>
+      <c r="D59" s="112"/>
+      <c r="E59" s="112"/>
+      <c r="F59" s="112"/>
+      <c r="G59" s="112"/>
+      <c r="H59" s="113"/>
     </row>
     <row r="60" spans="1:8" ht="140.25">
       <c r="A60" s="31" t="s">
@@ -4003,15 +4101,15 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="31"/>
-      <c r="B64" s="99" t="s">
+      <c r="B64" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="C64" s="100"/>
-      <c r="D64" s="100"/>
-      <c r="E64" s="100"/>
-      <c r="F64" s="100"/>
-      <c r="G64" s="100"/>
-      <c r="H64" s="101"/>
+      <c r="C64" s="112"/>
+      <c r="D64" s="112"/>
+      <c r="E64" s="112"/>
+      <c r="F64" s="112"/>
+      <c r="G64" s="112"/>
+      <c r="H64" s="113"/>
     </row>
     <row r="65" spans="1:8" ht="14.25" customHeight="1">
       <c r="A65" s="62" t="s">
@@ -4233,15 +4331,15 @@
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="31"/>
-      <c r="B76" s="93" t="s">
+      <c r="B76" s="102" t="s">
         <v>57</v>
       </c>
-      <c r="C76" s="94"/>
-      <c r="D76" s="94"/>
-      <c r="E76" s="94"/>
-      <c r="F76" s="94"/>
-      <c r="G76" s="94"/>
-      <c r="H76" s="95"/>
+      <c r="C76" s="103"/>
+      <c r="D76" s="103"/>
+      <c r="E76" s="103"/>
+      <c r="F76" s="103"/>
+      <c r="G76" s="103"/>
+      <c r="H76" s="104"/>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1">
       <c r="A77" s="57"/>
@@ -4371,15 +4469,15 @@
     </row>
     <row r="84" spans="1:8">
       <c r="A84" s="31"/>
-      <c r="B84" s="93" t="s">
+      <c r="B84" s="102" t="s">
         <v>72</v>
       </c>
-      <c r="C84" s="94"/>
-      <c r="D84" s="94"/>
-      <c r="E84" s="94"/>
-      <c r="F84" s="94"/>
-      <c r="G84" s="94"/>
-      <c r="H84" s="95"/>
+      <c r="C84" s="103"/>
+      <c r="D84" s="103"/>
+      <c r="E84" s="103"/>
+      <c r="F84" s="103"/>
+      <c r="G84" s="103"/>
+      <c r="H84" s="104"/>
     </row>
     <row r="85" spans="1:8" ht="102">
       <c r="A85" s="31"/>
@@ -4459,13 +4557,13 @@
     </row>
     <row r="91" spans="1:8">
       <c r="A91" s="31"/>
-      <c r="B91" s="117"/>
-      <c r="C91" s="118"/>
-      <c r="D91" s="118"/>
-      <c r="E91" s="118"/>
-      <c r="F91" s="118"/>
-      <c r="G91" s="118"/>
-      <c r="H91" s="119"/>
+      <c r="B91" s="105"/>
+      <c r="C91" s="106"/>
+      <c r="D91" s="106"/>
+      <c r="E91" s="106"/>
+      <c r="F91" s="106"/>
+      <c r="G91" s="106"/>
+      <c r="H91" s="107"/>
     </row>
     <row r="92" spans="1:8">
       <c r="A92" s="31"/>
@@ -4499,13 +4597,13 @@
     </row>
     <row r="95" spans="1:8">
       <c r="A95" s="31"/>
-      <c r="B95" s="90"/>
-      <c r="C95" s="91"/>
-      <c r="D95" s="91"/>
-      <c r="E95" s="91"/>
-      <c r="F95" s="91"/>
-      <c r="G95" s="91"/>
-      <c r="H95" s="92"/>
+      <c r="B95" s="96"/>
+      <c r="C95" s="97"/>
+      <c r="D95" s="97"/>
+      <c r="E95" s="97"/>
+      <c r="F95" s="97"/>
+      <c r="G95" s="97"/>
+      <c r="H95" s="98"/>
     </row>
     <row r="96" spans="1:8">
       <c r="A96" s="31"/>
@@ -4609,13 +4707,13 @@
     </row>
     <row r="106" spans="1:8">
       <c r="A106" s="31"/>
-      <c r="B106" s="114"/>
-      <c r="C106" s="115"/>
-      <c r="D106" s="115"/>
-      <c r="E106" s="115"/>
-      <c r="F106" s="115"/>
-      <c r="G106" s="115"/>
-      <c r="H106" s="116"/>
+      <c r="B106" s="99"/>
+      <c r="C106" s="100"/>
+      <c r="D106" s="100"/>
+      <c r="E106" s="100"/>
+      <c r="F106" s="100"/>
+      <c r="G106" s="100"/>
+      <c r="H106" s="101"/>
     </row>
     <row r="107" spans="1:8">
       <c r="A107" s="31"/>
@@ -4659,13 +4757,13 @@
     </row>
     <row r="111" spans="1:8">
       <c r="A111" s="31"/>
-      <c r="B111" s="111"/>
-      <c r="C111" s="112"/>
-      <c r="D111" s="112"/>
-      <c r="E111" s="112"/>
-      <c r="F111" s="112"/>
-      <c r="G111" s="112"/>
-      <c r="H111" s="113"/>
+      <c r="B111" s="93"/>
+      <c r="C111" s="94"/>
+      <c r="D111" s="94"/>
+      <c r="E111" s="94"/>
+      <c r="F111" s="94"/>
+      <c r="G111" s="94"/>
+      <c r="H111" s="95"/>
     </row>
     <row r="112" spans="1:8">
       <c r="A112" s="31"/>
@@ -4729,13 +4827,13 @@
     </row>
     <row r="118" spans="1:8">
       <c r="A118" s="31"/>
-      <c r="B118" s="105"/>
-      <c r="C118" s="106"/>
-      <c r="D118" s="106"/>
-      <c r="E118" s="106"/>
-      <c r="F118" s="106"/>
-      <c r="G118" s="106"/>
-      <c r="H118" s="107"/>
+      <c r="B118" s="90"/>
+      <c r="C118" s="91"/>
+      <c r="D118" s="91"/>
+      <c r="E118" s="91"/>
+      <c r="F118" s="91"/>
+      <c r="G118" s="91"/>
+      <c r="H118" s="92"/>
     </row>
     <row r="119" spans="1:8" ht="193.5" customHeight="1">
       <c r="A119" s="31"/>
@@ -4809,13 +4907,13 @@
     </row>
     <row r="126" spans="1:8" ht="13.5" customHeight="1">
       <c r="A126" s="31"/>
-      <c r="B126" s="105"/>
-      <c r="C126" s="106"/>
-      <c r="D126" s="106"/>
-      <c r="E126" s="106"/>
-      <c r="F126" s="106"/>
-      <c r="G126" s="106"/>
-      <c r="H126" s="107"/>
+      <c r="B126" s="90"/>
+      <c r="C126" s="91"/>
+      <c r="D126" s="91"/>
+      <c r="E126" s="91"/>
+      <c r="F126" s="91"/>
+      <c r="G126" s="91"/>
+      <c r="H126" s="92"/>
     </row>
     <row r="127" spans="1:8">
       <c r="A127" s="31"/>
@@ -4889,13 +4987,13 @@
     </row>
     <row r="134" spans="1:8" ht="13.5" customHeight="1">
       <c r="A134" s="31"/>
-      <c r="B134" s="105"/>
-      <c r="C134" s="106"/>
-      <c r="D134" s="106"/>
-      <c r="E134" s="106"/>
-      <c r="F134" s="106"/>
-      <c r="G134" s="106"/>
-      <c r="H134" s="107"/>
+      <c r="B134" s="90"/>
+      <c r="C134" s="91"/>
+      <c r="D134" s="91"/>
+      <c r="E134" s="91"/>
+      <c r="F134" s="91"/>
+      <c r="G134" s="91"/>
+      <c r="H134" s="92"/>
     </row>
     <row r="135" spans="1:8">
       <c r="A135" s="31"/>
@@ -4939,13 +5037,13 @@
     </row>
     <row r="139" spans="1:8" ht="12.75" customHeight="1">
       <c r="A139" s="31"/>
-      <c r="B139" s="105"/>
-      <c r="C139" s="106"/>
-      <c r="D139" s="106"/>
-      <c r="E139" s="106"/>
-      <c r="F139" s="106"/>
-      <c r="G139" s="106"/>
-      <c r="H139" s="107"/>
+      <c r="B139" s="90"/>
+      <c r="C139" s="91"/>
+      <c r="D139" s="91"/>
+      <c r="E139" s="91"/>
+      <c r="F139" s="91"/>
+      <c r="G139" s="91"/>
+      <c r="H139" s="92"/>
     </row>
     <row r="140" spans="1:8">
       <c r="A140" s="31"/>
@@ -5019,13 +5117,13 @@
     </row>
     <row r="147" spans="1:8" ht="12.75" customHeight="1">
       <c r="A147" s="31"/>
-      <c r="B147" s="90"/>
-      <c r="C147" s="91"/>
-      <c r="D147" s="91"/>
-      <c r="E147" s="91"/>
-      <c r="F147" s="91"/>
-      <c r="G147" s="91"/>
-      <c r="H147" s="92"/>
+      <c r="B147" s="96"/>
+      <c r="C147" s="97"/>
+      <c r="D147" s="97"/>
+      <c r="E147" s="97"/>
+      <c r="F147" s="97"/>
+      <c r="G147" s="97"/>
+      <c r="H147" s="98"/>
     </row>
     <row r="148" spans="1:8">
       <c r="A148" s="31"/>
@@ -5217,17 +5315,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B134:H134"/>
-    <mergeCell ref="B111:H111"/>
-    <mergeCell ref="B95:H95"/>
-    <mergeCell ref="B106:H106"/>
-    <mergeCell ref="B76:H76"/>
-    <mergeCell ref="B91:H91"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
     <mergeCell ref="B147:H147"/>
     <mergeCell ref="B28:H28"/>
     <mergeCell ref="B9:H9"/>
@@ -5241,6 +5328,17 @@
     <mergeCell ref="B118:H118"/>
     <mergeCell ref="B126:H126"/>
     <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B134:H134"/>
+    <mergeCell ref="B111:H111"/>
+    <mergeCell ref="B95:H95"/>
+    <mergeCell ref="B106:H106"/>
+    <mergeCell ref="B76:H76"/>
+    <mergeCell ref="B91:H91"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F3 F7:F8 F10:F13 F17:F27 F36 F65">
@@ -5252,4 +5350,1137 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H104"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="29" style="5" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B1" s="37"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="81"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" ht="26.25">
+      <c r="A3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="88"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="86" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="87"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A6" s="20">
+        <f>COUNTIF(F12:F661,"Pass")</f>
+        <v>0</v>
+      </c>
+      <c r="B6" s="21">
+        <f>COUNTIF(F12:F1108,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="21">
+        <f>E6-D6-B6-A6</f>
+        <v>11</v>
+      </c>
+      <c r="D6" s="22">
+        <f>COUNTIF(F$12:F$1108,"N/A")</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="79">
+        <f>COUNTIF($C12:$C168, "*")</f>
+        <v>11</v>
+      </c>
+      <c r="F6" s="80"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" ht="25.5">
+      <c r="A8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="11"/>
+      <c r="B9" s="108" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="109"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="110"/>
+    </row>
+    <row r="10" spans="1:8" ht="25.5">
+      <c r="A10" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>221</v>
+      </c>
+      <c r="E10" s="32"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="34"/>
+    </row>
+    <row r="11" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A11" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="51" t="s">
+        <v>215</v>
+      </c>
+      <c r="E11" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="F11" s="53"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="45"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="46"/>
+      <c r="B12" s="117" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="118"/>
+      <c r="D12" s="118"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="118"/>
+      <c r="G12" s="118"/>
+      <c r="H12" s="119"/>
+    </row>
+    <row r="13" spans="1:8" ht="25.5">
+      <c r="A13" s="62" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="47"/>
+      <c r="C13" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="49" t="s">
+        <v>226</v>
+      </c>
+      <c r="E13" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+    </row>
+    <row r="14" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A14" s="62" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="47"/>
+      <c r="C14" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="121" t="s">
+        <v>216</v>
+      </c>
+      <c r="E14" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+    </row>
+    <row r="15" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A15" s="62" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="47"/>
+      <c r="C15" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="121" t="s">
+        <v>217</v>
+      </c>
+      <c r="E15" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="F15" s="47"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+    </row>
+    <row r="16" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A16" s="62" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" s="47"/>
+      <c r="C16" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="121" t="s">
+        <v>218</v>
+      </c>
+      <c r="E16" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+    </row>
+    <row r="17" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A17" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" s="47"/>
+      <c r="C17" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="121" t="s">
+        <v>219</v>
+      </c>
+      <c r="E17" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+    </row>
+    <row r="18" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A18" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" s="47"/>
+      <c r="C18" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" s="121" t="s">
+        <v>220</v>
+      </c>
+      <c r="E18" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+    </row>
+    <row r="19" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A19" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="47"/>
+      <c r="C19" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="121" t="s">
+        <v>221</v>
+      </c>
+      <c r="E19" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+    </row>
+    <row r="20" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A20" s="62" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="47"/>
+      <c r="C20" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="121" t="s">
+        <v>222</v>
+      </c>
+      <c r="E20" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+    </row>
+    <row r="21" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A21" s="62" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" s="47"/>
+      <c r="C21" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="121" t="s">
+        <v>223</v>
+      </c>
+      <c r="E21" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+    </row>
+    <row r="22" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A22" s="62" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" s="47"/>
+      <c r="C22" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="121" t="s">
+        <v>224</v>
+      </c>
+      <c r="E22" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+    </row>
+    <row r="23" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A23" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" s="47"/>
+      <c r="C23" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="121" t="s">
+        <v>225</v>
+      </c>
+      <c r="E23" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="31"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="31"/>
+      <c r="B25" s="70"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="31"/>
+      <c r="B26" s="70"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="31"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+    </row>
+    <row r="28" spans="1:8" s="124" customFormat="1">
+      <c r="A28" s="122"/>
+      <c r="B28" s="123"/>
+      <c r="C28" s="123"/>
+      <c r="D28" s="123"/>
+      <c r="E28" s="123"/>
+      <c r="F28" s="123"/>
+      <c r="G28" s="123"/>
+      <c r="H28" s="123"/>
+    </row>
+    <row r="29" spans="1:8" s="124" customFormat="1">
+      <c r="A29" s="122"/>
+      <c r="B29" s="125"/>
+      <c r="C29" s="122"/>
+      <c r="D29" s="122"/>
+      <c r="E29" s="126"/>
+      <c r="F29" s="126"/>
+      <c r="G29" s="126"/>
+      <c r="H29" s="126"/>
+    </row>
+    <row r="30" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A30" s="122"/>
+      <c r="B30" s="125"/>
+      <c r="C30" s="122"/>
+      <c r="D30" s="122"/>
+      <c r="E30" s="126"/>
+      <c r="F30" s="126"/>
+      <c r="G30" s="126"/>
+      <c r="H30" s="126"/>
+    </row>
+    <row r="31" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A31" s="122"/>
+      <c r="B31" s="125"/>
+      <c r="C31" s="122"/>
+      <c r="D31" s="122"/>
+      <c r="E31" s="126"/>
+      <c r="F31" s="126"/>
+      <c r="G31" s="126"/>
+      <c r="H31" s="126"/>
+    </row>
+    <row r="32" spans="1:8" s="124" customFormat="1">
+      <c r="A32" s="122"/>
+      <c r="B32" s="127"/>
+      <c r="C32" s="127"/>
+      <c r="D32" s="127"/>
+      <c r="E32" s="127"/>
+      <c r="F32" s="127"/>
+      <c r="G32" s="127"/>
+      <c r="H32" s="127"/>
+    </row>
+    <row r="33" spans="1:8" s="124" customFormat="1">
+      <c r="A33" s="122"/>
+      <c r="B33" s="128"/>
+      <c r="C33" s="122"/>
+      <c r="D33" s="122"/>
+      <c r="E33" s="128"/>
+      <c r="F33" s="128"/>
+      <c r="G33" s="128"/>
+      <c r="H33" s="128"/>
+    </row>
+    <row r="34" spans="1:8" s="124" customFormat="1" ht="12" customHeight="1">
+      <c r="A34" s="122"/>
+      <c r="B34" s="128"/>
+      <c r="C34" s="122"/>
+      <c r="D34" s="122"/>
+      <c r="E34" s="128"/>
+      <c r="F34" s="128"/>
+      <c r="G34" s="128"/>
+      <c r="H34" s="128"/>
+    </row>
+    <row r="35" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A35" s="122"/>
+      <c r="B35" s="128"/>
+      <c r="C35" s="122"/>
+      <c r="D35" s="122"/>
+      <c r="E35" s="128"/>
+      <c r="F35" s="128"/>
+      <c r="G35" s="128"/>
+      <c r="H35" s="128"/>
+    </row>
+    <row r="36" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A36" s="122"/>
+      <c r="B36" s="128"/>
+      <c r="C36" s="122"/>
+      <c r="D36" s="122"/>
+      <c r="E36" s="128"/>
+      <c r="F36" s="128"/>
+      <c r="G36" s="128"/>
+      <c r="H36" s="128"/>
+    </row>
+    <row r="37" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A37" s="122"/>
+      <c r="B37" s="128"/>
+      <c r="C37" s="122"/>
+      <c r="D37" s="122"/>
+    </row>
+    <row r="38" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A38" s="122"/>
+      <c r="B38" s="128"/>
+      <c r="C38" s="122"/>
+      <c r="D38" s="122"/>
+    </row>
+    <row r="39" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A39" s="122"/>
+      <c r="B39" s="128"/>
+      <c r="C39" s="122"/>
+      <c r="D39" s="122"/>
+    </row>
+    <row r="40" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A40" s="122"/>
+      <c r="B40" s="128"/>
+      <c r="C40" s="122"/>
+      <c r="D40" s="122"/>
+    </row>
+    <row r="41" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A41" s="122"/>
+      <c r="B41" s="128"/>
+      <c r="C41" s="122"/>
+      <c r="D41" s="122"/>
+    </row>
+    <row r="42" spans="1:8" s="124" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A42" s="122"/>
+      <c r="B42" s="128"/>
+      <c r="C42" s="122"/>
+      <c r="D42" s="122"/>
+    </row>
+    <row r="43" spans="1:8" s="124" customFormat="1">
+      <c r="A43" s="122"/>
+      <c r="B43" s="127"/>
+      <c r="C43" s="127"/>
+      <c r="D43" s="127"/>
+      <c r="E43" s="127"/>
+      <c r="F43" s="127"/>
+      <c r="G43" s="127"/>
+      <c r="H43" s="127"/>
+    </row>
+    <row r="44" spans="1:8" s="124" customFormat="1">
+      <c r="A44" s="122"/>
+      <c r="B44" s="128"/>
+      <c r="C44" s="122"/>
+      <c r="D44" s="122"/>
+      <c r="E44" s="128"/>
+      <c r="F44" s="128"/>
+      <c r="G44" s="128"/>
+      <c r="H44" s="128"/>
+    </row>
+    <row r="45" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A45" s="122"/>
+      <c r="B45" s="128"/>
+      <c r="C45" s="122"/>
+      <c r="D45" s="122"/>
+    </row>
+    <row r="46" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A46" s="122"/>
+      <c r="B46" s="128"/>
+      <c r="C46" s="122"/>
+      <c r="D46" s="122"/>
+    </row>
+    <row r="47" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A47" s="122"/>
+      <c r="B47" s="128"/>
+      <c r="C47" s="122"/>
+      <c r="D47" s="122"/>
+    </row>
+    <row r="48" spans="1:8" s="124" customFormat="1">
+      <c r="A48" s="122"/>
+      <c r="B48" s="129"/>
+      <c r="C48" s="129"/>
+      <c r="D48" s="129"/>
+      <c r="E48" s="129"/>
+      <c r="F48" s="129"/>
+      <c r="G48" s="129"/>
+      <c r="H48" s="129"/>
+    </row>
+    <row r="49" spans="1:8" s="124" customFormat="1">
+      <c r="A49" s="122"/>
+      <c r="B49" s="128"/>
+      <c r="C49" s="122"/>
+      <c r="D49" s="122"/>
+    </row>
+    <row r="50" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A50" s="122"/>
+      <c r="B50" s="128"/>
+      <c r="C50" s="122"/>
+      <c r="D50" s="122"/>
+    </row>
+    <row r="51" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A51" s="122"/>
+      <c r="B51" s="128"/>
+      <c r="C51" s="122"/>
+      <c r="D51" s="122"/>
+    </row>
+    <row r="52" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A52" s="122"/>
+      <c r="B52" s="128"/>
+      <c r="C52" s="122"/>
+      <c r="D52" s="122"/>
+    </row>
+    <row r="53" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A53" s="122"/>
+      <c r="B53" s="128"/>
+      <c r="C53" s="122"/>
+      <c r="D53" s="122"/>
+    </row>
+    <row r="54" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A54" s="122"/>
+      <c r="B54" s="128"/>
+      <c r="C54" s="122"/>
+      <c r="D54" s="122"/>
+    </row>
+    <row r="55" spans="1:8" s="124" customFormat="1">
+      <c r="A55" s="122"/>
+      <c r="B55" s="129"/>
+      <c r="C55" s="129"/>
+      <c r="D55" s="129"/>
+      <c r="E55" s="129"/>
+      <c r="F55" s="129"/>
+      <c r="G55" s="129"/>
+      <c r="H55" s="129"/>
+    </row>
+    <row r="56" spans="1:8" s="124" customFormat="1" ht="193.5" customHeight="1">
+      <c r="A56" s="122"/>
+      <c r="B56" s="128"/>
+      <c r="C56" s="122"/>
+      <c r="D56" s="122"/>
+    </row>
+    <row r="57" spans="1:8" s="124" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A57" s="122"/>
+      <c r="B57" s="128"/>
+      <c r="C57" s="122"/>
+      <c r="D57" s="122"/>
+    </row>
+    <row r="58" spans="1:8" s="124" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A58" s="122"/>
+      <c r="B58" s="128"/>
+      <c r="C58" s="122"/>
+      <c r="D58" s="122"/>
+    </row>
+    <row r="59" spans="1:8" s="124" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A59" s="122"/>
+      <c r="B59" s="128"/>
+      <c r="C59" s="122"/>
+      <c r="D59" s="122"/>
+    </row>
+    <row r="60" spans="1:8" s="124" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A60" s="122"/>
+      <c r="B60" s="128"/>
+      <c r="C60" s="122"/>
+      <c r="D60" s="122"/>
+    </row>
+    <row r="61" spans="1:8" s="124" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A61" s="122"/>
+      <c r="B61" s="128"/>
+      <c r="C61" s="122"/>
+      <c r="D61" s="122"/>
+    </row>
+    <row r="62" spans="1:8" s="124" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A62" s="122"/>
+      <c r="B62" s="128"/>
+      <c r="C62" s="122"/>
+      <c r="D62" s="122"/>
+    </row>
+    <row r="63" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A63" s="122"/>
+      <c r="B63" s="129"/>
+      <c r="C63" s="129"/>
+      <c r="D63" s="129"/>
+      <c r="E63" s="129"/>
+      <c r="F63" s="129"/>
+      <c r="G63" s="129"/>
+      <c r="H63" s="129"/>
+    </row>
+    <row r="64" spans="1:8" s="124" customFormat="1">
+      <c r="A64" s="122"/>
+      <c r="B64" s="130"/>
+      <c r="C64" s="122"/>
+      <c r="D64" s="122"/>
+      <c r="E64" s="130"/>
+      <c r="F64" s="130"/>
+      <c r="G64" s="130"/>
+      <c r="H64" s="130"/>
+    </row>
+    <row r="65" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A65" s="122"/>
+      <c r="B65" s="130"/>
+      <c r="C65" s="122"/>
+      <c r="D65" s="122"/>
+      <c r="E65" s="130"/>
+      <c r="F65" s="130"/>
+      <c r="G65" s="130"/>
+      <c r="H65" s="130"/>
+    </row>
+    <row r="66" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A66" s="122"/>
+      <c r="B66" s="130"/>
+      <c r="C66" s="122"/>
+      <c r="D66" s="122"/>
+      <c r="E66" s="130"/>
+      <c r="F66" s="130"/>
+      <c r="G66" s="130"/>
+      <c r="H66" s="130"/>
+    </row>
+    <row r="67" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A67" s="122"/>
+      <c r="B67" s="130"/>
+      <c r="C67" s="122"/>
+      <c r="D67" s="122"/>
+      <c r="E67" s="130"/>
+      <c r="F67" s="130"/>
+      <c r="G67" s="130"/>
+      <c r="H67" s="130"/>
+    </row>
+    <row r="68" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A68" s="122"/>
+      <c r="B68" s="130"/>
+      <c r="C68" s="122"/>
+      <c r="D68" s="122"/>
+      <c r="E68" s="130"/>
+      <c r="F68" s="130"/>
+      <c r="G68" s="130"/>
+      <c r="H68" s="130"/>
+    </row>
+    <row r="69" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A69" s="122"/>
+      <c r="B69" s="130"/>
+      <c r="C69" s="122"/>
+      <c r="D69" s="122"/>
+      <c r="E69" s="130"/>
+      <c r="F69" s="130"/>
+      <c r="G69" s="130"/>
+      <c r="H69" s="130"/>
+    </row>
+    <row r="70" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A70" s="122"/>
+      <c r="B70" s="130"/>
+      <c r="C70" s="122"/>
+      <c r="D70" s="122"/>
+      <c r="E70" s="130"/>
+      <c r="F70" s="130"/>
+      <c r="G70" s="130"/>
+      <c r="H70" s="130"/>
+    </row>
+    <row r="71" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A71" s="122"/>
+      <c r="B71" s="129"/>
+      <c r="C71" s="129"/>
+      <c r="D71" s="129"/>
+      <c r="E71" s="129"/>
+      <c r="F71" s="129"/>
+      <c r="G71" s="129"/>
+      <c r="H71" s="129"/>
+    </row>
+    <row r="72" spans="1:8" s="124" customFormat="1">
+      <c r="A72" s="122"/>
+      <c r="B72" s="130"/>
+      <c r="C72" s="122"/>
+      <c r="D72" s="122"/>
+      <c r="E72" s="130"/>
+      <c r="F72" s="130"/>
+      <c r="G72" s="130"/>
+      <c r="H72" s="130"/>
+    </row>
+    <row r="73" spans="1:8" s="124" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A73" s="122"/>
+      <c r="B73" s="130"/>
+      <c r="C73" s="122"/>
+      <c r="D73" s="122"/>
+      <c r="E73" s="130"/>
+      <c r="F73" s="130"/>
+      <c r="G73" s="130"/>
+      <c r="H73" s="130"/>
+    </row>
+    <row r="74" spans="1:8" s="124" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A74" s="122"/>
+      <c r="B74" s="130"/>
+      <c r="C74" s="122"/>
+      <c r="D74" s="122"/>
+      <c r="E74" s="130"/>
+      <c r="F74" s="130"/>
+      <c r="G74" s="130"/>
+      <c r="H74" s="130"/>
+    </row>
+    <row r="75" spans="1:8" s="124" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A75" s="122"/>
+      <c r="B75" s="130"/>
+      <c r="C75" s="122"/>
+      <c r="D75" s="122"/>
+      <c r="E75" s="130"/>
+      <c r="F75" s="130"/>
+      <c r="G75" s="130"/>
+      <c r="H75" s="130"/>
+    </row>
+    <row r="76" spans="1:8" s="124" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A76" s="122"/>
+      <c r="B76" s="129"/>
+      <c r="C76" s="129"/>
+      <c r="D76" s="129"/>
+      <c r="E76" s="129"/>
+      <c r="F76" s="129"/>
+      <c r="G76" s="129"/>
+      <c r="H76" s="129"/>
+    </row>
+    <row r="77" spans="1:8" s="124" customFormat="1">
+      <c r="A77" s="122"/>
+      <c r="B77" s="130"/>
+      <c r="C77" s="122"/>
+      <c r="D77" s="122"/>
+      <c r="E77" s="130"/>
+      <c r="F77" s="130"/>
+      <c r="G77" s="130"/>
+      <c r="H77" s="130"/>
+    </row>
+    <row r="78" spans="1:8" s="124" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A78" s="122"/>
+      <c r="B78" s="130"/>
+      <c r="C78" s="122"/>
+      <c r="D78" s="122"/>
+      <c r="E78" s="130"/>
+      <c r="F78" s="130"/>
+      <c r="G78" s="130"/>
+      <c r="H78" s="130"/>
+    </row>
+    <row r="79" spans="1:8" s="124" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A79" s="122"/>
+      <c r="B79" s="130"/>
+      <c r="C79" s="122"/>
+      <c r="D79" s="122"/>
+      <c r="E79" s="130"/>
+      <c r="F79" s="130"/>
+      <c r="G79" s="130"/>
+      <c r="H79" s="130"/>
+    </row>
+    <row r="80" spans="1:8" s="124" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A80" s="122"/>
+      <c r="B80" s="130"/>
+      <c r="C80" s="122"/>
+      <c r="D80" s="122"/>
+      <c r="E80" s="130"/>
+      <c r="F80" s="130"/>
+      <c r="G80" s="130"/>
+      <c r="H80" s="130"/>
+    </row>
+    <row r="81" spans="1:8" s="124" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A81" s="122"/>
+      <c r="B81" s="130"/>
+      <c r="C81" s="122"/>
+      <c r="D81" s="122"/>
+      <c r="E81" s="130"/>
+      <c r="F81" s="130"/>
+      <c r="G81" s="130"/>
+      <c r="H81" s="130"/>
+    </row>
+    <row r="82" spans="1:8" s="124" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A82" s="122"/>
+      <c r="B82" s="130"/>
+      <c r="C82" s="122"/>
+      <c r="D82" s="122"/>
+      <c r="E82" s="130"/>
+      <c r="F82" s="130"/>
+      <c r="G82" s="130"/>
+      <c r="H82" s="130"/>
+    </row>
+    <row r="83" spans="1:8" s="124" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A83" s="122"/>
+      <c r="B83" s="130"/>
+      <c r="C83" s="122"/>
+      <c r="D83" s="122"/>
+      <c r="E83" s="130"/>
+      <c r="F83" s="130"/>
+      <c r="G83" s="130"/>
+      <c r="H83" s="130"/>
+    </row>
+    <row r="84" spans="1:8" s="124" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A84" s="122"/>
+      <c r="B84" s="127"/>
+      <c r="C84" s="127"/>
+      <c r="D84" s="127"/>
+      <c r="E84" s="127"/>
+      <c r="F84" s="127"/>
+      <c r="G84" s="127"/>
+      <c r="H84" s="127"/>
+    </row>
+    <row r="85" spans="1:8" s="124" customFormat="1">
+      <c r="A85" s="122"/>
+      <c r="B85" s="130"/>
+      <c r="C85" s="122"/>
+      <c r="D85" s="122"/>
+      <c r="E85" s="130"/>
+      <c r="F85" s="130"/>
+      <c r="G85" s="130"/>
+      <c r="H85" s="130"/>
+    </row>
+    <row r="86" spans="1:8" s="124" customFormat="1" ht="144" customHeight="1">
+      <c r="A86" s="122"/>
+      <c r="B86" s="130"/>
+      <c r="C86" s="122"/>
+      <c r="D86" s="122"/>
+      <c r="E86" s="130"/>
+      <c r="F86" s="130"/>
+      <c r="G86" s="130"/>
+      <c r="H86" s="130"/>
+    </row>
+    <row r="87" spans="1:8" s="124" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A87" s="122"/>
+      <c r="B87" s="130"/>
+      <c r="C87" s="122"/>
+      <c r="D87" s="122"/>
+      <c r="E87" s="130"/>
+      <c r="F87" s="130"/>
+      <c r="G87" s="130"/>
+      <c r="H87" s="130"/>
+    </row>
+    <row r="88" spans="1:8" s="124" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A88" s="122"/>
+      <c r="B88" s="130"/>
+      <c r="C88" s="122"/>
+      <c r="D88" s="122"/>
+      <c r="E88" s="130"/>
+      <c r="F88" s="130"/>
+      <c r="G88" s="130"/>
+      <c r="H88" s="130"/>
+    </row>
+    <row r="89" spans="1:8" s="124" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A89" s="122"/>
+      <c r="B89" s="130"/>
+      <c r="C89" s="122"/>
+      <c r="D89" s="122"/>
+      <c r="E89" s="130"/>
+      <c r="F89" s="130"/>
+      <c r="G89" s="130"/>
+      <c r="H89" s="130"/>
+    </row>
+    <row r="90" spans="1:8" s="124" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A90" s="122"/>
+      <c r="B90" s="130"/>
+      <c r="C90" s="122"/>
+      <c r="D90" s="122"/>
+      <c r="E90" s="130"/>
+      <c r="F90" s="130"/>
+      <c r="G90" s="130"/>
+      <c r="H90" s="130"/>
+    </row>
+    <row r="91" spans="1:8" s="124" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A91" s="122"/>
+      <c r="B91" s="130"/>
+      <c r="C91" s="122"/>
+      <c r="D91" s="122"/>
+      <c r="E91" s="130"/>
+      <c r="F91" s="130"/>
+      <c r="G91" s="130"/>
+      <c r="H91" s="130"/>
+    </row>
+    <row r="92" spans="1:8" s="124" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A92" s="122"/>
+      <c r="B92" s="130"/>
+      <c r="C92" s="122"/>
+      <c r="D92" s="122"/>
+      <c r="E92" s="130"/>
+      <c r="F92" s="130"/>
+      <c r="G92" s="130"/>
+      <c r="H92" s="130"/>
+    </row>
+    <row r="93" spans="1:8" s="124" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A93" s="122"/>
+      <c r="B93" s="130"/>
+      <c r="C93" s="122"/>
+      <c r="D93" s="122"/>
+      <c r="E93" s="130"/>
+      <c r="F93" s="130"/>
+      <c r="G93" s="130"/>
+      <c r="H93" s="130"/>
+    </row>
+    <row r="94" spans="1:8" s="124" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A94" s="122"/>
+      <c r="B94" s="130"/>
+      <c r="C94" s="122"/>
+      <c r="D94" s="122"/>
+      <c r="E94" s="130"/>
+      <c r="F94" s="130"/>
+      <c r="G94" s="130"/>
+      <c r="H94" s="130"/>
+    </row>
+    <row r="95" spans="1:8" s="124" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A95" s="122"/>
+      <c r="B95" s="130"/>
+      <c r="C95" s="122"/>
+      <c r="D95" s="122"/>
+      <c r="E95" s="130"/>
+      <c r="F95" s="130"/>
+      <c r="G95" s="130"/>
+      <c r="H95" s="130"/>
+    </row>
+    <row r="96" spans="1:8" s="124" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A96" s="122"/>
+      <c r="B96" s="130"/>
+      <c r="C96" s="122"/>
+      <c r="D96" s="122"/>
+      <c r="E96" s="130"/>
+      <c r="F96" s="130"/>
+      <c r="G96" s="130"/>
+      <c r="H96" s="130"/>
+    </row>
+    <row r="97" spans="1:8" s="124" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A97" s="122"/>
+      <c r="B97" s="130"/>
+      <c r="C97" s="122"/>
+      <c r="D97" s="122"/>
+      <c r="E97" s="130"/>
+      <c r="F97" s="130"/>
+      <c r="G97" s="130"/>
+      <c r="H97" s="130"/>
+    </row>
+    <row r="98" spans="1:8" s="124" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A98" s="122"/>
+      <c r="B98" s="130"/>
+      <c r="C98" s="122"/>
+      <c r="D98" s="122"/>
+      <c r="E98" s="130"/>
+      <c r="F98" s="130"/>
+      <c r="G98" s="130"/>
+      <c r="H98" s="130"/>
+    </row>
+    <row r="99" spans="1:8" s="124" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A99" s="122"/>
+      <c r="B99" s="130"/>
+      <c r="C99" s="122"/>
+      <c r="D99" s="122"/>
+      <c r="E99" s="130"/>
+      <c r="F99" s="130"/>
+      <c r="G99" s="130"/>
+      <c r="H99" s="130"/>
+    </row>
+    <row r="100" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A100" s="122"/>
+      <c r="B100" s="130"/>
+      <c r="C100" s="122"/>
+      <c r="D100" s="122"/>
+      <c r="E100" s="130"/>
+      <c r="F100" s="130"/>
+      <c r="G100" s="130"/>
+      <c r="H100" s="130"/>
+    </row>
+    <row r="101" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A101" s="122"/>
+      <c r="B101" s="130"/>
+      <c r="C101" s="130"/>
+      <c r="D101" s="130"/>
+      <c r="E101" s="130"/>
+      <c r="F101" s="130"/>
+      <c r="G101" s="130"/>
+      <c r="H101" s="130"/>
+    </row>
+    <row r="102" spans="1:8" s="124" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A102" s="122"/>
+      <c r="B102" s="128"/>
+      <c r="C102" s="130"/>
+      <c r="D102" s="130"/>
+    </row>
+    <row r="103" spans="1:8" s="124" customFormat="1">
+      <c r="C103" s="122"/>
+      <c r="D103" s="122"/>
+    </row>
+    <row r="104" spans="1:8" s="124" customFormat="1">
+      <c r="C104" s="122"/>
+      <c r="D104" s="122"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="B48:H48"/>
+    <mergeCell ref="B55:H55"/>
+    <mergeCell ref="B63:H63"/>
+    <mergeCell ref="B71:H71"/>
+    <mergeCell ref="B76:H76"/>
+    <mergeCell ref="B84:H84"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B9:H9"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F3 F7:F8 F13:F23 F10:F11">
+      <formula1>$J$2:$J$6</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>